<commit_message>
updated the testcases for Duplicate and Data comparison to take count in query instead of Snowflake fetchSize Method
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ServiceTitan_ColumnValidation_Snowflake.xlsx
+++ b/src/test/resources/TestData/ServiceTitan_ColumnValidation_Snowflake.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balamurugan.t\git\DF_Automation_Framework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AD74CD-A875-4103-80EB-ECAF86E3955E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BAD488-47AB-44A7-850C-6AACFB8D5845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18855" uniqueCount="1488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18855" uniqueCount="1489">
   <si>
     <t>TC_ID</t>
   </si>
@@ -4504,7 +4504,10 @@
     <t>BKPOnly_Table</t>
   </si>
   <si>
-    <t>N</t>
+    <t>SHIFT</t>
+  </si>
+  <si>
+    <t>APPOINTMENT</t>
   </si>
 </sst>
 </file>
@@ -5103,8 +5106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6C016F-FCBC-41FF-84E1-C3AC17BABEE6}">
   <dimension ref="A1:J1189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J1189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5591,7 +5594,7 @@
         <v>98</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -5625,7 +5628,7 @@
         <v>99</v>
       </c>
       <c r="J15" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -5659,7 +5662,7 @@
         <v>97</v>
       </c>
       <c r="J16" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -6169,7 +6172,7 @@
         <v>98</v>
       </c>
       <c r="J31" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -6203,7 +6206,7 @@
         <v>99</v>
       </c>
       <c r="J32" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -6237,7 +6240,7 @@
         <v>97</v>
       </c>
       <c r="J33" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
@@ -6747,7 +6750,7 @@
         <v>98</v>
       </c>
       <c r="J48" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
@@ -6781,7 +6784,7 @@
         <v>99</v>
       </c>
       <c r="J49" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -6815,7 +6818,7 @@
         <v>97</v>
       </c>
       <c r="J50" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -7325,7 +7328,7 @@
         <v>98</v>
       </c>
       <c r="J65" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
@@ -7359,7 +7362,7 @@
         <v>99</v>
       </c>
       <c r="J66" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
@@ -7393,7 +7396,7 @@
         <v>97</v>
       </c>
       <c r="J67" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
@@ -7903,7 +7906,7 @@
         <v>98</v>
       </c>
       <c r="J82" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
@@ -7937,7 +7940,7 @@
         <v>99</v>
       </c>
       <c r="J83" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
@@ -7971,7 +7974,7 @@
         <v>97</v>
       </c>
       <c r="J84" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
@@ -8481,7 +8484,7 @@
         <v>98</v>
       </c>
       <c r="J99" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
@@ -8515,7 +8518,7 @@
         <v>99</v>
       </c>
       <c r="J100" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
@@ -8549,7 +8552,7 @@
         <v>97</v>
       </c>
       <c r="J101" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
@@ -9059,7 +9062,7 @@
         <v>98</v>
       </c>
       <c r="J116" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.35">
@@ -9093,7 +9096,7 @@
         <v>99</v>
       </c>
       <c r="J117" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.35">
@@ -9127,7 +9130,7 @@
         <v>97</v>
       </c>
       <c r="J118" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
@@ -9637,7 +9640,7 @@
         <v>98</v>
       </c>
       <c r="J133" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.35">
@@ -9671,7 +9674,7 @@
         <v>99</v>
       </c>
       <c r="J134" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.35">
@@ -9705,7 +9708,7 @@
         <v>97</v>
       </c>
       <c r="J135" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.35">
@@ -10215,7 +10218,7 @@
         <v>98</v>
       </c>
       <c r="J150" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.35">
@@ -10249,7 +10252,7 @@
         <v>99</v>
       </c>
       <c r="J151" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.35">
@@ -10283,7 +10286,7 @@
         <v>97</v>
       </c>
       <c r="J152" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.35">
@@ -10793,7 +10796,7 @@
         <v>98</v>
       </c>
       <c r="J167" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.35">
@@ -10827,7 +10830,7 @@
         <v>99</v>
       </c>
       <c r="J168" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.35">
@@ -10861,7 +10864,7 @@
         <v>97</v>
       </c>
       <c r="J169" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.35">
@@ -11371,7 +11374,7 @@
         <v>98</v>
       </c>
       <c r="J184" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.35">
@@ -11405,7 +11408,7 @@
         <v>99</v>
       </c>
       <c r="J185" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.35">
@@ -11439,7 +11442,7 @@
         <v>97</v>
       </c>
       <c r="J186" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.35">
@@ -11949,7 +11952,7 @@
         <v>98</v>
       </c>
       <c r="J201" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.35">
@@ -11983,7 +11986,7 @@
         <v>99</v>
       </c>
       <c r="J202" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.35">
@@ -12017,7 +12020,7 @@
         <v>97</v>
       </c>
       <c r="J203" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.35">
@@ -12960,7 +12963,7 @@
         <v>439</v>
       </c>
       <c r="G231" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H231" s="23" t="s">
         <v>427</v>
@@ -13309,7 +13312,7 @@
         <v>96</v>
       </c>
       <c r="J241" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.35">
@@ -13334,7 +13337,7 @@
         <v>439</v>
       </c>
       <c r="G242" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H242" s="23" t="s">
         <v>431</v>
@@ -13343,7 +13346,7 @@
         <v>420</v>
       </c>
       <c r="J242" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.35">
@@ -14354,7 +14357,7 @@
         <v>439</v>
       </c>
       <c r="G272" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H272" s="23" t="s">
         <v>427</v>
@@ -14703,7 +14706,7 @@
         <v>96</v>
       </c>
       <c r="J282" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.35">
@@ -14728,7 +14731,7 @@
         <v>439</v>
       </c>
       <c r="G283" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H283" s="23" t="s">
         <v>431</v>
@@ -14737,7 +14740,7 @@
         <v>420</v>
       </c>
       <c r="J283" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.35">
@@ -15748,7 +15751,7 @@
         <v>439</v>
       </c>
       <c r="G313" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H313" s="23" t="s">
         <v>427</v>
@@ -16097,7 +16100,7 @@
         <v>96</v>
       </c>
       <c r="J323" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.35">
@@ -16122,7 +16125,7 @@
         <v>439</v>
       </c>
       <c r="G324" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H324" s="23" t="s">
         <v>431</v>
@@ -16131,7 +16134,7 @@
         <v>420</v>
       </c>
       <c r="J324" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.35">
@@ -17142,7 +17145,7 @@
         <v>439</v>
       </c>
       <c r="G354" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H354" s="23" t="s">
         <v>427</v>
@@ -17491,7 +17494,7 @@
         <v>96</v>
       </c>
       <c r="J364" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="365" spans="1:10" x14ac:dyDescent="0.35">
@@ -17516,7 +17519,7 @@
         <v>439</v>
       </c>
       <c r="G365" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H365" s="23" t="s">
         <v>431</v>
@@ -17525,7 +17528,7 @@
         <v>420</v>
       </c>
       <c r="J365" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="366" spans="1:10" x14ac:dyDescent="0.35">
@@ -18536,7 +18539,7 @@
         <v>439</v>
       </c>
       <c r="G395" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H395" s="23" t="s">
         <v>427</v>
@@ -18885,7 +18888,7 @@
         <v>96</v>
       </c>
       <c r="J405" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="406" spans="1:10" x14ac:dyDescent="0.35">
@@ -18910,7 +18913,7 @@
         <v>439</v>
       </c>
       <c r="G406" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H406" s="23" t="s">
         <v>431</v>
@@ -18919,7 +18922,7 @@
         <v>420</v>
       </c>
       <c r="J406" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="407" spans="1:10" x14ac:dyDescent="0.35">
@@ -19930,7 +19933,7 @@
         <v>439</v>
       </c>
       <c r="G436" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H436" s="23" t="s">
         <v>427</v>
@@ -20279,7 +20282,7 @@
         <v>96</v>
       </c>
       <c r="J446" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="447" spans="1:10" x14ac:dyDescent="0.35">
@@ -20304,7 +20307,7 @@
         <v>439</v>
       </c>
       <c r="G447" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H447" s="23" t="s">
         <v>431</v>
@@ -20313,7 +20316,7 @@
         <v>420</v>
       </c>
       <c r="J447" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="448" spans="1:10" x14ac:dyDescent="0.35">
@@ -21324,7 +21327,7 @@
         <v>439</v>
       </c>
       <c r="G477" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H477" s="23" t="s">
         <v>427</v>
@@ -21673,7 +21676,7 @@
         <v>96</v>
       </c>
       <c r="J487" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="488" spans="1:10" x14ac:dyDescent="0.35">
@@ -21698,7 +21701,7 @@
         <v>439</v>
       </c>
       <c r="G488" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H488" s="23" t="s">
         <v>431</v>
@@ -21707,7 +21710,7 @@
         <v>420</v>
       </c>
       <c r="J488" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="489" spans="1:10" x14ac:dyDescent="0.35">
@@ -22718,7 +22721,7 @@
         <v>439</v>
       </c>
       <c r="G518" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H518" s="23" t="s">
         <v>427</v>
@@ -23067,7 +23070,7 @@
         <v>96</v>
       </c>
       <c r="J528" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="529" spans="1:10" x14ac:dyDescent="0.35">
@@ -23092,7 +23095,7 @@
         <v>439</v>
       </c>
       <c r="G529" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H529" s="23" t="s">
         <v>431</v>
@@ -23101,7 +23104,7 @@
         <v>420</v>
       </c>
       <c r="J529" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="530" spans="1:10" x14ac:dyDescent="0.35">
@@ -24112,7 +24115,7 @@
         <v>439</v>
       </c>
       <c r="G559" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H559" s="23" t="s">
         <v>427</v>
@@ -24461,7 +24464,7 @@
         <v>96</v>
       </c>
       <c r="J569" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="570" spans="1:10" x14ac:dyDescent="0.35">
@@ -24486,7 +24489,7 @@
         <v>439</v>
       </c>
       <c r="G570" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H570" s="23" t="s">
         <v>431</v>
@@ -24495,7 +24498,7 @@
         <v>420</v>
       </c>
       <c r="J570" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="571" spans="1:10" x14ac:dyDescent="0.35">
@@ -25506,7 +25509,7 @@
         <v>439</v>
       </c>
       <c r="G600" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H600" s="23" t="s">
         <v>427</v>
@@ -25855,7 +25858,7 @@
         <v>96</v>
       </c>
       <c r="J610" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="611" spans="1:10" x14ac:dyDescent="0.35">
@@ -25880,7 +25883,7 @@
         <v>439</v>
       </c>
       <c r="G611" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H611" s="23" t="s">
         <v>431</v>
@@ -25889,7 +25892,7 @@
         <v>420</v>
       </c>
       <c r="J611" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="612" spans="1:10" x14ac:dyDescent="0.35">
@@ -26900,7 +26903,7 @@
         <v>439</v>
       </c>
       <c r="G641" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H641" s="23" t="s">
         <v>427</v>
@@ -27249,7 +27252,7 @@
         <v>96</v>
       </c>
       <c r="J651" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="652" spans="1:10" x14ac:dyDescent="0.35">
@@ -27274,7 +27277,7 @@
         <v>439</v>
       </c>
       <c r="G652" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H652" s="23" t="s">
         <v>431</v>
@@ -27283,7 +27286,7 @@
         <v>420</v>
       </c>
       <c r="J652" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="653" spans="1:10" x14ac:dyDescent="0.35">
@@ -28294,7 +28297,7 @@
         <v>439</v>
       </c>
       <c r="G682" s="23" t="s">
-        <v>426</v>
+        <v>1488</v>
       </c>
       <c r="H682" s="23" t="s">
         <v>427</v>
@@ -28643,7 +28646,7 @@
         <v>96</v>
       </c>
       <c r="J692" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="693" spans="1:10" x14ac:dyDescent="0.35">
@@ -28668,7 +28671,7 @@
         <v>439</v>
       </c>
       <c r="G693" s="23" t="s">
-        <v>430</v>
+        <v>1487</v>
       </c>
       <c r="H693" s="23" t="s">
         <v>431</v>
@@ -28677,7 +28680,7 @@
         <v>420</v>
       </c>
       <c r="J693" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="694" spans="1:10" x14ac:dyDescent="0.35">
@@ -30001,7 +30004,7 @@
         <v>96</v>
       </c>
       <c r="J733" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="734" spans="1:10" x14ac:dyDescent="0.35">
@@ -30034,7 +30037,7 @@
         <v>420</v>
       </c>
       <c r="J734" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="735" spans="1:10" x14ac:dyDescent="0.35">
@@ -31354,7 +31357,7 @@
         <v>96</v>
       </c>
       <c r="J774" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="775" spans="1:10" x14ac:dyDescent="0.35">
@@ -31387,7 +31390,7 @@
         <v>420</v>
       </c>
       <c r="J775" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="776" spans="1:10" x14ac:dyDescent="0.35">
@@ -32707,7 +32710,7 @@
         <v>96</v>
       </c>
       <c r="J815" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="816" spans="1:10" x14ac:dyDescent="0.35">
@@ -32740,7 +32743,7 @@
         <v>420</v>
       </c>
       <c r="J816" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="817" spans="1:10" x14ac:dyDescent="0.35">
@@ -34060,7 +34063,7 @@
         <v>96</v>
       </c>
       <c r="J856" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="857" spans="1:10" x14ac:dyDescent="0.35">
@@ -34093,7 +34096,7 @@
         <v>420</v>
       </c>
       <c r="J857" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="858" spans="1:10" x14ac:dyDescent="0.35">
@@ -35413,7 +35416,7 @@
         <v>96</v>
       </c>
       <c r="J897" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="898" spans="1:10" x14ac:dyDescent="0.35">
@@ -35446,7 +35449,7 @@
         <v>420</v>
       </c>
       <c r="J898" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="899" spans="1:10" x14ac:dyDescent="0.35">
@@ -36766,7 +36769,7 @@
         <v>96</v>
       </c>
       <c r="J938" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="939" spans="1:10" x14ac:dyDescent="0.35">
@@ -36799,7 +36802,7 @@
         <v>420</v>
       </c>
       <c r="J939" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="940" spans="1:10" x14ac:dyDescent="0.35">
@@ -38119,7 +38122,7 @@
         <v>96</v>
       </c>
       <c r="J979" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="980" spans="1:10" x14ac:dyDescent="0.35">
@@ -38152,7 +38155,7 @@
         <v>420</v>
       </c>
       <c r="J980" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="981" spans="1:10" x14ac:dyDescent="0.35">
@@ -39472,7 +39475,7 @@
         <v>96</v>
       </c>
       <c r="J1020" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1021" spans="1:10" x14ac:dyDescent="0.35">
@@ -39505,7 +39508,7 @@
         <v>420</v>
       </c>
       <c r="J1021" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1022" spans="1:10" x14ac:dyDescent="0.35">
@@ -40825,7 +40828,7 @@
         <v>96</v>
       </c>
       <c r="J1061" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1062" spans="1:10" x14ac:dyDescent="0.35">
@@ -40858,7 +40861,7 @@
         <v>420</v>
       </c>
       <c r="J1062" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1063" spans="1:10" x14ac:dyDescent="0.35">
@@ -42178,7 +42181,7 @@
         <v>96</v>
       </c>
       <c r="J1102" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1103" spans="1:10" x14ac:dyDescent="0.35">
@@ -42211,7 +42214,7 @@
         <v>420</v>
       </c>
       <c r="J1103" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1104" spans="1:10" x14ac:dyDescent="0.35">
@@ -43531,7 +43534,7 @@
         <v>96</v>
       </c>
       <c r="J1143" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1144" spans="1:10" x14ac:dyDescent="0.35">
@@ -43564,7 +43567,7 @@
         <v>420</v>
       </c>
       <c r="J1144" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1145" spans="1:10" x14ac:dyDescent="0.35">
@@ -44884,7 +44887,7 @@
         <v>96</v>
       </c>
       <c r="J1184" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1185" spans="1:10" x14ac:dyDescent="0.35">
@@ -44917,7 +44920,7 @@
         <v>420</v>
       </c>
       <c r="J1185" s="29" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1186" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>